<commit_message>
Ready for turn in.
</commit_message>
<xml_diff>
--- a/Project2/p6.xlsx
+++ b/Project2/p6.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="p6" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -3167,11 +3167,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="521923960"/>
-        <c:axId val="521922000"/>
+        <c:axId val="713419424"/>
+        <c:axId val="713416680"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="521923960"/>
+        <c:axId val="713419424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3270,7 +3270,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="521922000"/>
+        <c:crossAx val="713416680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3278,7 +3278,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="521922000"/>
+        <c:axId val="713416680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3385,7 +3385,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="521923960"/>
+        <c:crossAx val="713419424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6139,11 +6139,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="522725008"/>
-        <c:axId val="522728144"/>
+        <c:axId val="713417856"/>
+        <c:axId val="713424520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="522725008"/>
+        <c:axId val="713417856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6242,7 +6242,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="522728144"/>
+        <c:crossAx val="713424520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6250,7 +6250,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="522728144"/>
+        <c:axId val="713424520"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -6363,7 +6363,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="522725008"/>
+        <c:crossAx val="713417856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7886,13 +7886,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E202"/>
+  <dimension ref="A1:E205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V35" sqref="V35"/>
+    <sheetView tabSelected="1" topLeftCell="A191" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G201" sqref="G201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -11326,6 +11331,16 @@
       </c>
       <c r="E202">
         <v>74</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B205" s="1">
+        <f>AVERAGE(B2:B202)</f>
+        <v>2.0625635630475619E-5</v>
+      </c>
+      <c r="D205" s="1">
+        <f>AVERAGE(D2:D202)</f>
+        <v>1.453354012192587E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>